<commit_message>
update to some overall formatting
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,8 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1904643312396bbe/Documents/GitHub/Senior-Capstone/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_CEDEFA3665894F2B8AD22A78DD2D3AB4104E24E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7642CD03-18F7-415F-B4E2-98B0EF8C2D77}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -11,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Branch Num</t>
   </si>
@@ -75,12 +84,856 @@
 </sst>
 </file>
 
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="33">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+  </fills>
+  <borders count="10">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="42">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office 2013 - 2022">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office 2013 - 2022">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office 2013 - 2022">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="2C7EE24B-C535-494D-AA97-0A61EE84BA40">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="63.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -91,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>142</v>
       </c>
@@ -102,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>150</v>
       </c>
@@ -113,7 +966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>131</v>
       </c>
@@ -124,7 +977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>43</v>
       </c>
@@ -135,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>33</v>
       </c>
@@ -146,7 +999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>114</v>
       </c>
@@ -157,7 +1010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>66</v>
       </c>
@@ -168,7 +1021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>67</v>
       </c>
@@ -179,7 +1032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>125</v>
       </c>
@@ -190,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>152</v>
       </c>
@@ -201,7 +1054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>153</v>
       </c>
@@ -212,7 +1065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>123</v>
       </c>
@@ -223,7 +1076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>124</v>
       </c>
@@ -234,7 +1087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>85</v>
       </c>
@@ -245,7 +1098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>86</v>
       </c>
@@ -256,7 +1109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>165</v>
       </c>
@@ -267,7 +1120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>166</v>
       </c>
@@ -278,7 +1131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>168</v>
       </c>
@@ -289,7 +1142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>163</v>
       </c>
@@ -300,7 +1153,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>164</v>
       </c>
@@ -311,7 +1164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17</v>
       </c>
@@ -322,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>92</v>
       </c>
@@ -333,7 +1186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>102</v>
       </c>
@@ -344,7 +1197,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>72</v>
       </c>
@@ -355,7 +1208,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.25" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>73</v>
       </c>

</xml_diff>